<commit_message>
admin service has almost done
</commit_message>
<xml_diff>
--- a/admin/data/round.xlsx
+++ b/admin/data/round.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3">
   <si>
     <t>round</t>
   </si>
   <si>
     <t>prizeid</t>
+  </si>
+  <si>
+    <t>level</t>
   </si>
 </sst>
 </file>
@@ -27,9 +30,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -42,31 +45,16 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -78,16 +66,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -101,6 +120,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -110,16 +144,23 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -127,44 +168,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -194,187 +197,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,15 +396,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -430,17 +424,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -455,6 +443,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -490,148 +493,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -958,276 +961,375 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="B1" sqref="B$1:B$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>501</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
         <v>502</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
         <v>503</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
         <v>504</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6">
         <v>505</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7">
         <v>506</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8">
         <v>507</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
         <v>508</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10">
         <v>509</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11">
         <v>510</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12">
         <v>401</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13">
         <v>402</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14">
         <v>403</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15">
         <v>404</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16">
         <v>405</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17">
         <v>406</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18">
         <v>407</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19">
         <v>301</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>4</v>
       </c>
       <c r="B20">
         <v>302</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>5</v>
       </c>
       <c r="B21">
         <v>303</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>6</v>
       </c>
       <c r="B22">
         <v>304</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>7</v>
       </c>
       <c r="B23">
         <v>305</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>8</v>
       </c>
       <c r="B24">
         <v>306</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>9</v>
       </c>
       <c r="B25">
         <v>201</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>10</v>
       </c>
       <c r="B26">
         <v>202</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>11</v>
       </c>
       <c r="B27">
         <v>203</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>12</v>
       </c>
       <c r="B28">
         <v>204</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>13</v>
       </c>
       <c r="B29">
         <v>205</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>14</v>
       </c>
       <c r="B30">
         <v>101</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>15</v>
       </c>
       <c r="B31">
         <v>102</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>16</v>
       </c>
       <c r="B32">
         <v>103</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>17</v>
       </c>
       <c r="B33">
         <v>104</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>